<commit_message>
Updated FRA model - 2025-08-07 13:55
</commit_message>
<xml_diff>
--- a/VerveStacks_FRA/SuppXLS/Scen_Par-NGFS.xlsx
+++ b/VerveStacks_FRA/SuppXLS/Scen_Par-NGFS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_FRA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{106C8531-FCA8-4AF7-A191-F773C6E8E70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{36ED6724-5CD3-4224-8CC2-D51CAB0453AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -753,25 +753,25 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>484.28000000000003</c:v>
+                  <c:v>469.34</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>525.79702362085879</c:v>
+                  <c:v>509.5762266998716</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>560.44327220587127</c:v>
+                  <c:v>543.15364123462371</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>547.46920232435286</c:v>
+                  <c:v>530.57982039091371</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>571.40727492264728</c:v>
+                  <c:v>553.77940532789955</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>638.28769149498157</c:v>
+                  <c:v>618.59656629688311</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>687.07750358463522</c:v>
+                  <c:v>665.88121651196127</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2783,7 +2783,7 @@
   <dimension ref="B2:AA34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2852,8 +2852,8 @@
         <v>3</v>
       </c>
       <c r="Q10" s="3">
-        <f>SUMIFS(historical_data_long!$D$3:$D$9999,historical_data_long!$B$3:$B$9999,Veda!Q9,historical_data_long!$C$3:$C$9999,"TWh")</f>
-        <v>484.28000000000003</v>
+        <f>SUMIFS(historical_data_long!$D$3:$D$9999,historical_data_long!$B$3:$B$9999,Veda!Q9,historical_data_long!$C$3:$C$9999,"TWh")-R25+R26</f>
+        <v>469.34000000000003</v>
       </c>
       <c r="R10" s="2" t="s">
         <v>16</v>
@@ -2876,31 +2876,31 @@
       </c>
       <c r="R12" s="8">
         <f>SUM(R16:R19)</f>
-        <v>484.28000000000003</v>
+        <v>469.34</v>
       </c>
       <c r="S12" s="8">
         <f t="shared" ref="S12:X12" si="0">SUM(S16:S19)</f>
-        <v>525.79702362085879</v>
+        <v>509.5762266998716</v>
       </c>
       <c r="T12" s="8">
         <f t="shared" si="0"/>
-        <v>560.44327220587127</v>
+        <v>543.15364123462371</v>
       </c>
       <c r="U12" s="8">
         <f t="shared" si="0"/>
-        <v>547.46920232435286</v>
+        <v>530.57982039091371</v>
       </c>
       <c r="V12" s="8">
         <f t="shared" si="0"/>
-        <v>571.40727492264728</v>
+        <v>553.77940532789955</v>
       </c>
       <c r="W12" s="8">
         <f t="shared" si="0"/>
-        <v>638.28769149498157</v>
+        <v>618.59656629688311</v>
       </c>
       <c r="X12" s="8">
         <f t="shared" si="0"/>
-        <v>687.07750358463522</v>
+        <v>665.88121651196127</v>
       </c>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.45">
@@ -3006,31 +3006,31 @@
       </c>
       <c r="R16" s="6">
         <f>$Q$10*G16/SUM($G$16:$G$18)</f>
-        <v>19.917938268809898</v>
+        <v>19.303471436118027</v>
       </c>
       <c r="S16" s="6">
         <f>R16</f>
-        <v>19.917938268809898</v>
+        <v>19.303471436118027</v>
       </c>
       <c r="T16" s="6">
         <f t="shared" ref="T16:X16" si="2">S16</f>
-        <v>19.917938268809898</v>
+        <v>19.303471436118027</v>
       </c>
       <c r="U16" s="6">
         <f t="shared" si="2"/>
-        <v>19.917938268809898</v>
+        <v>19.303471436118027</v>
       </c>
       <c r="V16" s="6">
         <f t="shared" si="2"/>
-        <v>19.917938268809898</v>
+        <v>19.303471436118027</v>
       </c>
       <c r="W16" s="6">
         <f t="shared" si="2"/>
-        <v>19.917938268809898</v>
+        <v>19.303471436118027</v>
       </c>
       <c r="X16" s="6">
         <f t="shared" si="2"/>
-        <v>19.917938268809898</v>
+        <v>19.303471436118027</v>
       </c>
       <c r="Y16" t="s">
         <v>11</v>
@@ -3073,31 +3073,31 @@
       </c>
       <c r="R17" s="6">
         <f>$Q$10*G17/SUM($G$16:$G$18)</f>
-        <v>379.86614746056904</v>
+        <v>368.14730661836842</v>
       </c>
       <c r="S17" s="6">
         <f t="shared" ref="S17:X18" si="3">R17*H17/G17</f>
-        <v>420.87151762131157</v>
+        <v>407.88766432722053</v>
       </c>
       <c r="T17" s="6">
         <f t="shared" si="3"/>
-        <v>462.53472794506075</v>
+        <v>448.26556788166926</v>
       </c>
       <c r="U17" s="6">
         <f t="shared" si="3"/>
-        <v>459.06279375141497</v>
+        <v>444.90074258546514</v>
       </c>
       <c r="V17" s="6">
         <f t="shared" si="3"/>
-        <v>482.92777299826423</v>
+        <v>468.02948909516243</v>
       </c>
       <c r="W17" s="6">
         <f t="shared" si="3"/>
-        <v>539.02692023243537</v>
+        <v>522.39798203909129</v>
       </c>
       <c r="X17" s="6">
         <f t="shared" si="3"/>
-        <v>568.95864764923408</v>
+        <v>551.40631801373468</v>
       </c>
       <c r="Y17" t="s">
         <v>11</v>
@@ -3137,31 +3137,31 @@
       </c>
       <c r="R18" s="6">
         <f>$Q$10*G18/SUM($G$16:$G$18)</f>
-        <v>84.495914270621071</v>
+        <v>81.88922194551354</v>
       </c>
       <c r="S18" s="6">
         <f t="shared" si="3"/>
-        <v>85.519221190853514</v>
+        <v>82.880959927552652</v>
       </c>
       <c r="T18" s="6">
         <f t="shared" si="3"/>
-        <v>73.166444796619118</v>
+        <v>70.909265715795044</v>
       </c>
       <c r="U18" s="6">
         <f t="shared" si="3"/>
-        <v>69.255950494302326</v>
+        <v>67.119409855859956</v>
       </c>
       <c r="V18" s="6">
         <f t="shared" si="3"/>
-        <v>73.276084823786888</v>
+        <v>71.015523356727826</v>
       </c>
       <c r="W18" s="6">
         <f t="shared" si="3"/>
-        <v>79.781393102407364</v>
+        <v>77.320143385404904</v>
       </c>
       <c r="X18" s="6">
         <f t="shared" si="3"/>
-        <v>82.924407214549845</v>
+        <v>80.36619575881069</v>
       </c>
       <c r="Y18" t="s">
         <v>11</v>
@@ -3180,27 +3180,27 @@
       </c>
       <c r="S19" s="6">
         <f t="shared" ref="S19:X19" si="4">$Q$10*H16/SUM($G$16:$G$18)-S16</f>
-        <v>-0.51165346011621438</v>
+        <v>-0.49586899101954529</v>
       </c>
       <c r="T19" s="6">
         <f t="shared" si="4"/>
-        <v>4.8241611953814783</v>
+        <v>4.6753362010414286</v>
       </c>
       <c r="U19" s="6">
         <f t="shared" si="4"/>
-        <v>-0.76748019017432156</v>
+        <v>-0.74380348652931971</v>
       </c>
       <c r="V19" s="6">
         <f t="shared" si="4"/>
-        <v>-4.714521168213718</v>
+        <v>-4.5690785601086716</v>
       </c>
       <c r="W19" s="6">
         <f t="shared" si="4"/>
-        <v>-0.43856010867104445</v>
+        <v>-0.42503056373103831</v>
       </c>
       <c r="X19" s="6">
         <f t="shared" si="4"/>
-        <v>15.276510452041357</v>
+        <v>14.805231303297862</v>
       </c>
       <c r="Y19" t="s">
         <v>11</v>

</xml_diff>